<commit_message>
Code for SNR analysis and statistics.
</commit_message>
<xml_diff>
--- a/Data/Results from Final project, 12-9.xlsx
+++ b/Data/Results from Final project, 12-9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\NENR_FinalPjt\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5743890F-DC3D-4C12-A086-F9C0D51CA367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0EF7C7-38B1-45E1-BBD4-09F13303D112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC6DA994-8028-F549-B3A8-9CFC684B706B}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A2:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E2"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -436,13 +436,13 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
         <v>3</v>
       </c>
       <c r="G2" t="s">
@@ -501,10 +501,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6">
@@ -515,8 +515,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7">
         <v>5.43</v>
       </c>
@@ -525,8 +525,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
       <c r="C8">
         <v>4.9000000000000004</v>
       </c>
@@ -535,8 +535,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2">
         <v>2</v>
       </c>
       <c r="C9">
@@ -547,8 +547,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10">
         <v>11.92</v>
       </c>
@@ -557,8 +557,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="C11">
         <v>9.5</v>
       </c>
@@ -567,8 +567,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2">
         <v>3</v>
       </c>
       <c r="C12">
@@ -579,8 +579,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13">
         <v>10.99</v>
       </c>
@@ -589,8 +589,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="C14">
         <v>11.36</v>
       </c>
@@ -599,10 +599,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15">
@@ -613,8 +613,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16">
         <v>9.4600000000000009</v>
       </c>
@@ -623,8 +623,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17">
         <v>6.6</v>
       </c>
@@ -633,8 +633,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2">
         <v>2</v>
       </c>
       <c r="C18">
@@ -645,8 +645,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19">
         <v>8.01</v>
       </c>
@@ -655,8 +655,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20">
         <v>13.49</v>
       </c>
@@ -665,8 +665,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2">
         <v>3</v>
       </c>
       <c r="C21">
@@ -677,8 +677,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="C22">
         <v>11.89</v>
       </c>
@@ -687,8 +687,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="C23">
         <v>18.04</v>
       </c>
@@ -697,10 +697,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>3</v>
-      </c>
-      <c r="B24" s="1">
+      <c r="A24" s="2">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24">
@@ -711,8 +711,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25">
         <v>5.44</v>
       </c>
@@ -721,8 +721,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
       <c r="C26">
         <v>10.48</v>
       </c>
@@ -731,8 +731,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2">
         <v>2</v>
       </c>
       <c r="C27">
@@ -743,8 +743,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
       <c r="C28">
         <v>6.84</v>
       </c>
@@ -753,8 +753,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
       <c r="C29">
         <v>7.5</v>
       </c>
@@ -763,8 +763,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2">
         <v>3</v>
       </c>
       <c r="C30">
@@ -775,8 +775,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31">
         <v>13.13</v>
       </c>
@@ -785,8 +785,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
       <c r="C32">
         <v>11.9</v>
       </c>
@@ -889,7 +889,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6">
@@ -903,7 +903,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2"/>
       <c r="B7">
         <v>2</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2"/>
       <c r="B8">
         <v>3</v>
       </c>
@@ -927,7 +927,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
       <c r="B9">
         <v>1</v>
       </c>
@@ -939,7 +939,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
       <c r="B10">
         <v>3</v>
       </c>
@@ -951,7 +951,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11">
         <v>2</v>
       </c>
@@ -963,7 +963,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2"/>
       <c r="B12">
         <v>2</v>
       </c>
@@ -975,7 +975,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="2"/>
       <c r="B13">
         <v>1</v>
       </c>
@@ -987,7 +987,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="2"/>
       <c r="B14">
         <v>3</v>
       </c>
@@ -999,7 +999,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>2</v>
       </c>
       <c r="B15">
@@ -1013,7 +1013,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="2"/>
       <c r="B16">
         <v>2</v>
       </c>
@@ -1025,7 +1025,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="2"/>
       <c r="B17">
         <v>3</v>
       </c>
@@ -1037,7 +1037,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2"/>
       <c r="B18">
         <v>1</v>
       </c>
@@ -1049,7 +1049,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2"/>
       <c r="B19">
         <v>2</v>
       </c>
@@ -1061,7 +1061,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="2"/>
       <c r="B20">
         <v>3</v>
       </c>
@@ -1073,7 +1073,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="2"/>
       <c r="B21">
         <v>2</v>
       </c>
@@ -1085,7 +1085,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="2"/>
       <c r="B22">
         <v>1</v>
       </c>
@@ -1097,7 +1097,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="2"/>
       <c r="B23">
         <v>1</v>
       </c>
@@ -1109,10 +1109,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>3</v>
-      </c>
-      <c r="B24" s="1">
+      <c r="A24" s="2">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24">
@@ -1123,8 +1123,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25">
         <v>5.44</v>
       </c>
@@ -1133,8 +1133,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
       <c r="C26">
         <v>10.48</v>
       </c>
@@ -1143,8 +1143,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2">
         <v>2</v>
       </c>
       <c r="C27">
@@ -1155,8 +1155,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
       <c r="C28">
         <v>6.84</v>
       </c>
@@ -1165,8 +1165,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
       <c r="C29">
         <v>7.5</v>
       </c>
@@ -1175,8 +1175,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2">
         <v>3</v>
       </c>
       <c r="C30">
@@ -1187,8 +1187,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31">
         <v>13.13</v>
       </c>
@@ -1197,8 +1197,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
       <c r="C32">
         <v>11.9</v>
       </c>

</xml_diff>